<commit_message>
v1.3.0 fix grammar excel
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/grammar/0624.xlsx
+++ b/ai/assets/textbook/grammar/0624.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\grammar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A8304-87CC-4950-8355-8EF1780234CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858AF3D8-5336-4523-A00C-84E13D516D79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="27390" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22230" yWindow="1710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$A$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$A$85</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -48,9 +48,6 @@
     <t>{77}dui dui dui W{77}</t>
   </si>
   <si>
-    <t>丁752丁丁福的</t>
-  </si>
-  <si>
     <t>{52}dui dui dui W{52}</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>{88} dui dui duiK{88}</t>
   </si>
   <si>
-    <t>人满开车打丁丁468丁</t>
-  </si>
-  <si>
     <t>{{65}vip vip vip R{65}</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
   </si>
   <si>
     <t>{65}vip vip vip X{65}</t>
-  </si>
-  <si>
-    <t>{74}{74} 丁丁468丁 {55}{55}</t>
   </si>
   <si>
     <t>{75}{76} why her nice</t>
@@ -145,17 +136,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>丁丁468丁{65}</t>
-  </si>
-  <si>
     <t>卫bei xu niu</t>
-  </si>
-  <si>
-    <t>146 连起来</t>
-  </si>
-  <si>
-    <t>丁丁468丁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -493,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -515,7 +496,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -523,7 +504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -531,7 +512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -539,7 +520,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -547,7 +528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -555,7 +536,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -563,7 +544,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -571,7 +552,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -579,7 +560,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -587,7 +568,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -595,7 +576,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -603,7 +584,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -611,7 +592,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -619,7 +600,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -627,7 +608,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -635,7 +616,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -643,7 +624,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -651,7 +632,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -659,7 +640,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -667,7 +648,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -675,7 +656,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -683,7 +664,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -691,7 +672,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -699,7 +680,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -707,7 +688,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -715,7 +696,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -723,7 +704,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -731,7 +712,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -739,7 +720,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -747,7 +728,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -755,7 +736,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -763,7 +744,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -777,58 +758,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:A91" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A40">
-      <sortCondition ref="A1:A91"/>
+  <autoFilter ref="A1:A85" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A34">
+      <sortCondition ref="A1:A85"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>